<commit_message>
fix: merge cell model
</commit_message>
<xml_diff>
--- a/src/containers/Excel/__tests__/origin.xlsx
+++ b/src/containers/Excel/__tests__/origin.xlsx
@@ -4,25 +4,32 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="11460"/>
+    <workbookView windowWidth="27660" windowHeight="11340" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>1a</t>
   </si>
   <si>
     <t>large text</t>
+  </si>
+  <si>
+    <t>1
+3
+2
+4</t>
   </si>
 </sst>
 </file>
@@ -665,9 +672,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1950,7 +1963,7 @@
   <sheetPr/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1990,42 +2003,42 @@
   </cols>
   <sheetData>
     <row r="1" ht="52" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>15</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2076,4 +2089,40 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B2:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="6:7">
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="6:7">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="F7:G8"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>